<commit_message>
Over ons + personeel toegevoegd
</commit_message>
<xml_diff>
--- a/Logboek/Logboek.xlsx
+++ b/Logboek/Logboek.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chris_dobvamy\Documents\GitHub\rijschool-abc\Logboek\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3309B05-143E-497F-9C4A-C41D1F07B4D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B134A546-95C6-4455-B955-88EDC251F9EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="65">
   <si>
     <t>Wat ga je vandaag doen?</t>
   </si>
@@ -202,6 +202,24 @@
   </si>
   <si>
     <t>Vandaag ga ik beginnen met het stylen van de login en aanmelden pagina's en het optimaliseren van afbeeldingen.</t>
+  </si>
+  <si>
+    <t>Vorige week vrijdag ben ik op zoek gegaan naar afbeeldingen en begonnen met het schrijven van teksten.</t>
+  </si>
+  <si>
+    <t>Vandaag wil ik de huisstyling + content op iedere pagina nalopen/afmaken. Daarnaast ga ik met Chris de login stylen.</t>
+  </si>
+  <si>
+    <t>Vandaag ga ik verder met het maken van de agenda voor de overzicht pagina's.</t>
+  </si>
+  <si>
+    <t>Vorige week vrijdag heb ik de tarieven pagina gestyled.</t>
+  </si>
+  <si>
+    <t>Vorige week vrijdag heb ik alle afbeeldingen geoptimaliseerd, de teksten toegevoegd en begonnen met het stylen van de login pagina.</t>
+  </si>
+  <si>
+    <t>Vandaag ga ik met Bruno op alle pagina's de huisstyling en content nalopen en de login stylen. En we gaan een blok maken met de medewerkers op de over ons pagina.</t>
   </si>
 </sst>
 </file>
@@ -592,9 +610,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F32"/>
+  <dimension ref="A1:F36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
       <selection activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
@@ -1072,6 +1090,62 @@
         <v>16</v>
       </c>
     </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="5">
+        <v>45376</v>
+      </c>
+      <c r="B33" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="C33" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="D33" s="9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A34" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B34" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="C34" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="D34" s="8" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A35" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B35" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="C35" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="D35" s="8" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B36" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="C36" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="D36" s="8" t="s">
+        <v>16</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>

</xml_diff>

<commit_message>
Comments + logboek update
Comments toegevoegd bij 404, home en extra pagina's + logboek geupdate.
</commit_message>
<xml_diff>
--- a/Logboek/Logboek.xlsx
+++ b/Logboek/Logboek.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chris_dobvamy\Documents\GitHub\rijschool-abc\Logboek\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC048CCD-77C5-49B3-B045-7275F8BE0132}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6246DEFB-5EEB-40AE-8E95-6B45B349C72B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="87">
   <si>
     <t>Wat ga je vandaag doen?</t>
   </si>
@@ -271,6 +271,21 @@
   </si>
   <si>
     <t>Vandaag ga ik een nieuw blok toevoegen aan de over ons pagina.</t>
+  </si>
+  <si>
+    <t>Vandaag hebben we de sprint review.</t>
+  </si>
+  <si>
+    <t>Vorige week heb ik een nieuw blok met auto's toegevoegd aan de over ons pagina.</t>
+  </si>
+  <si>
+    <t>Vorige week heb ik de login en aanmelden pagina's vertaald naar het Nederlands.</t>
+  </si>
+  <si>
+    <t>Vandaag ben ik ziek.</t>
+  </si>
+  <si>
+    <t>Vorige week donderdag was ik ziek.</t>
   </si>
 </sst>
 </file>
@@ -659,10 +674,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AXW48"/>
+  <dimension ref="A1:AXW52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
-      <selection activeCell="D47" sqref="D47"/>
+    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
+      <selection activeCell="D50" sqref="D50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13069,7 +13084,9 @@
       <c r="C47" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="D47" s="6"/>
+      <c r="D47" s="6" t="s">
+        <v>85</v>
+      </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
@@ -13082,6 +13099,62 @@
         <v>16</v>
       </c>
       <c r="D48" s="6" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A49" s="4">
+        <v>45384</v>
+      </c>
+      <c r="B49" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="C49" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="D49" s="7" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A50" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B50" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="C50" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="D50" s="6" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A51" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B51" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="C51" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="D51" s="6" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A52" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B52" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="C52" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D52" s="6" t="s">
         <v>32</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Logboek update + hero aanpassingen
</commit_message>
<xml_diff>
--- a/Logboek/Logboek.xlsx
+++ b/Logboek/Logboek.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chris_dobvamy\Documents\GitHub\rijschool-abc\Logboek\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32BF73BB-46E7-4156-935A-939301A98A98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33191DA6-A51F-4B91-BB00-DAE00700DC2F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="108">
   <si>
     <t>Wat ga je vandaag doen?</t>
   </si>
@@ -327,10 +327,28 @@
     <t>Gisteren heb ik de retrospective gemaakt en de readme aangepast.</t>
   </si>
   <si>
-    <t>Vandaag ga ik kijken of het database goed staat en deze bijwerken.</t>
+    <t>N.v.t.</t>
   </si>
   <si>
-    <t>N.v.t.</t>
+    <t>Vandaag ga ik kijken of het database goed staat en deze bijwerken. Daarnaast ga ik de retrospective afmaken.</t>
+  </si>
+  <si>
+    <t>Gisteren heb ik de retrospective afgemaakt.</t>
+  </si>
+  <si>
+    <t>Gisteren heb ik het contactformulier afgemaakt en de banner verbeterd.</t>
+  </si>
+  <si>
+    <t>Gisteren ben ik verder gegaan met het stylen van de overzichtspagina.</t>
+  </si>
+  <si>
+    <t>Ik heb hulp nodig van de docent bij het stylen van de overzichtspagina.</t>
+  </si>
+  <si>
+    <t>Vandaag ga ik met Chris de hero banner stylen.</t>
+  </si>
+  <si>
+    <t>Vandaag ga ik met Bruno de hero banner stylen.</t>
   </si>
 </sst>
 </file>
@@ -732,10 +750,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AXW62"/>
+  <dimension ref="A1:AXW67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="B61" sqref="B61"/>
+    <sheetView tabSelected="1" topLeftCell="A51" workbookViewId="0">
+      <selection activeCell="F61" sqref="F61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13319,7 +13337,7 @@
         <v>0</v>
       </c>
       <c r="B60" s="6" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C60" s="6" t="s">
         <v>96</v>
@@ -13333,7 +13351,7 @@
         <v>87</v>
       </c>
       <c r="B61" s="6" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C61" s="10" t="s">
         <v>94</v>
@@ -13354,6 +13372,76 @@
       </c>
       <c r="D62" s="6" t="s">
         <v>32</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A63" s="4">
+        <v>45387</v>
+      </c>
+      <c r="B63" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="C63" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="D63" s="7" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A64" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B64" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="C64" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="D64" s="6" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A65" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B65" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="C65" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="D65" s="6" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A66" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B66" s="10" t="s">
+        <v>88</v>
+      </c>
+      <c r="C66" s="10" t="s">
+        <v>88</v>
+      </c>
+      <c r="D66" s="10" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A67" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B67" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="C67" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D67" s="6" t="s">
+        <v>105</v>
       </c>
     </row>
   </sheetData>
@@ -13363,8 +13451,11 @@
     <hyperlink ref="B56" r:id="rId3" xr:uid="{B92C1E9A-1654-427D-B44D-A860E7699512}"/>
     <hyperlink ref="C61" r:id="rId4" xr:uid="{BA8F35F4-DF64-4F30-9F1B-82BBC53D0FC2}"/>
     <hyperlink ref="D61" r:id="rId5" xr:uid="{B8AB0389-6A31-4C87-8C26-CEF9A6FF7D72}"/>
+    <hyperlink ref="C66" r:id="rId6" xr:uid="{4F736914-BE59-4FA8-A64B-1A208F53BB95}"/>
+    <hyperlink ref="D66" r:id="rId7" xr:uid="{E6FCA577-14D0-4F63-AA31-A5F32A7973D9}"/>
+    <hyperlink ref="B66" r:id="rId8" xr:uid="{6160A85A-7656-499E-BB70-558330A0EB5F}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId6"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId9"/>
 </worksheet>
 </file>
</xml_diff>